<commit_message>
labour work for W3 partly done
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
+++ b/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="249">
   <si>
     <t>LevelName</t>
   </si>
@@ -363,9 +363,6 @@
     <t>MesoCarrier + Core</t>
   </si>
   <si>
-    <t>NewBoss</t>
-  </si>
-  <si>
     <t>HyperCarrier</t>
   </si>
   <si>
@@ -495,9 +492,6 @@
     <t>All basic available</t>
   </si>
   <si>
-    <t>Mix</t>
-  </si>
-  <si>
     <t>NanoBomb, MicroBomb</t>
   </si>
   <si>
@@ -754,6 +748,24 @@
   </si>
   <si>
     <t>10,11,15,16,25,26,30</t>
+  </si>
+  <si>
+    <t>Ernesto</t>
+  </si>
+  <si>
+    <t>Maxima</t>
+  </si>
+  <si>
+    <t>Max Couplad</t>
+  </si>
+  <si>
+    <t>Hyper Carrier &amp; Core</t>
+  </si>
+  <si>
+    <t>2 Couplad types</t>
+  </si>
+  <si>
+    <t>Gigantodon</t>
   </si>
 </sst>
 </file>
@@ -1198,9 +1210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1233,7 +1245,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>108</v>
@@ -1242,10 +1254,10 @@
         <v>2</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>155</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>156</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="21"/>
@@ -1262,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="12" t="s">
@@ -1288,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
@@ -1309,14 +1321,14 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H4" s="17">
         <v>100</v>
@@ -1333,14 +1345,14 @@
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H5" s="17">
         <v>100</v>
@@ -1356,17 +1368,17 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H6" s="17">
         <v>110</v>
@@ -1383,14 +1395,14 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H7" s="17">
         <v>110</v>
@@ -1406,17 +1418,17 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H8" s="17">
         <v>110</v>
@@ -1433,14 +1445,14 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H9" s="17">
         <v>120</v>
@@ -1457,14 +1469,14 @@
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H10" s="17">
         <v>120</v>
@@ -1481,16 +1493,16 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H11" s="17">
         <v>500</v>
@@ -1507,14 +1519,14 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H12" s="17">
         <v>130</v>
@@ -1531,14 +1543,14 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H13" s="17">
         <v>130</v>
@@ -1555,14 +1567,14 @@
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H14" s="17">
         <v>130</v>
@@ -1578,17 +1590,17 @@
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H15" s="17">
         <v>130</v>
@@ -1605,14 +1617,14 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H16" s="17">
         <v>140</v>
@@ -1629,14 +1641,14 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H17" s="17">
         <v>140</v>
@@ -1653,14 +1665,14 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H18" s="17">
         <v>140</v>
@@ -1677,14 +1689,14 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H19" s="17">
         <v>140</v>
@@ -1701,14 +1713,14 @@
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H20" s="17">
         <v>140</v>
@@ -1724,19 +1736,19 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H21" s="17">
         <v>500</v>
@@ -1753,14 +1765,14 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H22" s="17">
         <v>150</v>
@@ -1777,14 +1789,14 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H23" s="17">
         <v>150</v>
@@ -1801,14 +1813,14 @@
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H24" s="17">
         <v>150</v>
@@ -1825,14 +1837,14 @@
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H25" s="17">
         <v>150</v>
@@ -1849,16 +1861,16 @@
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H26" s="17">
         <v>700</v>
@@ -1874,17 +1886,17 @@
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H27" s="26">
         <v>120</v>
@@ -1901,14 +1913,14 @@
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
       <c r="D28" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H28" s="26">
         <v>120</v>
@@ -1925,14 +1937,14 @@
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H29" s="26">
         <v>120</v>
@@ -1949,14 +1961,14 @@
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H30" s="26">
         <v>120</v>
@@ -1973,10 +1985,10 @@
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="25"/>
@@ -1994,17 +2006,17 @@
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H32" s="26">
         <v>120</v>
@@ -2021,10 +2033,10 @@
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
       <c r="D33" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="25"/>
@@ -2043,10 +2055,10 @@
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
       <c r="D34" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="25"/>
@@ -2064,17 +2076,17 @@
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H35" s="26">
         <v>130</v>
@@ -2091,16 +2103,16 @@
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E36" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="G36" s="25" t="s">
         <v>235</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="G36" s="25" t="s">
-        <v>237</v>
       </c>
       <c r="H36" s="26">
         <v>500</v>
@@ -2116,17 +2128,17 @@
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H37" s="26">
         <v>150</v>
@@ -2143,10 +2155,10 @@
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
       <c r="D38" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="25"/>
@@ -2165,10 +2177,10 @@
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
       <c r="D39" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="25"/>
@@ -2187,10 +2199,10 @@
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="25"/>
@@ -2209,10 +2221,10 @@
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>111</v>
@@ -2232,17 +2244,17 @@
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H42" s="26">
         <v>160</v>
@@ -2259,10 +2271,10 @@
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="25"/>
@@ -2281,13 +2293,13 @@
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
       <c r="D44" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G44" s="25"/>
       <c r="H44" s="26">
@@ -2305,10 +2317,10 @@
       <c r="B45" s="23"/>
       <c r="C45" s="23"/>
       <c r="D45" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="25"/>
@@ -2327,10 +2339,10 @@
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>112</v>
@@ -2351,10 +2363,10 @@
       <c r="B47" s="23"/>
       <c r="C47" s="23"/>
       <c r="D47" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="25"/>
@@ -2373,10 +2385,10 @@
       <c r="B48" s="23"/>
       <c r="C48" s="23"/>
       <c r="D48" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="25"/>
@@ -2395,10 +2407,10 @@
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
       <c r="D49" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="25"/>
@@ -2417,10 +2429,10 @@
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
       <c r="D50" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="25"/>
@@ -2439,10 +2451,10 @@
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
       <c r="D51" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>113</v>
@@ -2463,10 +2475,10 @@
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
       <c r="D52" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="25"/>
@@ -2485,10 +2497,10 @@
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
       <c r="D53" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="25"/>
@@ -2507,10 +2519,10 @@
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
       <c r="D54" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="25"/>
@@ -2529,10 +2541,10 @@
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
       <c r="D55" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="25"/>
@@ -2551,13 +2563,13 @@
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
       <c r="D56" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="26">
@@ -2575,7 +2587,7 @@
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -2594,7 +2606,7 @@
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="14"/>
@@ -2613,7 +2625,7 @@
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -2632,7 +2644,7 @@
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="14"/>
@@ -2651,7 +2663,7 @@
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -2670,7 +2682,7 @@
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
       <c r="D62" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="14"/>
@@ -2689,7 +2701,7 @@
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
       <c r="D63" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -2708,7 +2720,7 @@
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="14"/>
@@ -2727,7 +2739,7 @@
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -2746,11 +2758,11 @@
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="14" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="18">
@@ -2767,7 +2779,7 @@
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
@@ -2786,7 +2798,7 @@
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="14"/>
@@ -2803,13 +2815,13 @@
         <v>74</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E69" s="13"/>
       <c r="F69" s="14"/>
@@ -2828,13 +2840,13 @@
         <v>75</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E70" s="13"/>
       <c r="F70" s="14"/>
@@ -2853,14 +2865,14 @@
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E71" s="13"/>
       <c r="F71" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H71" s="18">
         <v>1000</v>
@@ -2876,12 +2888,12 @@
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="14"/>
       <c r="G72" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H72" s="18">
         <v>450</v>
@@ -2897,12 +2909,12 @@
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="14"/>
       <c r="G73" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H73" s="18">
         <v>450</v>
@@ -2918,12 +2930,12 @@
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E74" s="13"/>
       <c r="F74" s="14"/>
       <c r="G74" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H74" s="18">
         <v>450</v>
@@ -2939,12 +2951,12 @@
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="14"/>
       <c r="G75" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H75" s="18">
         <v>450</v>
@@ -2960,14 +2972,14 @@
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H76" s="18">
         <v>1300</v>
@@ -2983,12 +2995,12 @@
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="14"/>
       <c r="G77" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H77" s="18">
         <v>450</v>
@@ -3004,12 +3016,12 @@
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
       <c r="D78" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="14"/>
       <c r="G78" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H78" s="18">
         <v>450</v>
@@ -3025,12 +3037,12 @@
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="14"/>
       <c r="G79" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H79" s="18">
         <v>450</v>
@@ -3046,12 +3058,12 @@
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
       <c r="D80" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="14"/>
       <c r="G80" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H80" s="18">
         <v>450</v>
@@ -3067,14 +3079,14 @@
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
       <c r="D81" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="14" t="s">
-        <v>114</v>
+        <v>248</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H81" s="18">
         <v>1800</v>
@@ -3090,12 +3102,12 @@
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="14"/>
       <c r="G82" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H82" s="18">
         <v>500</v>
@@ -3111,12 +3123,12 @@
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
       <c r="D83" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="14"/>
       <c r="G83" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H83" s="18">
         <v>500</v>
@@ -3132,12 +3144,12 @@
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
       <c r="D84" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E84" s="13"/>
       <c r="F84" s="14"/>
       <c r="G84" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H84" s="18">
         <v>500</v>
@@ -3153,12 +3165,12 @@
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="14"/>
       <c r="G85" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H85" s="18">
         <v>500</v>
@@ -3174,12 +3186,12 @@
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="14"/>
       <c r="G86" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H86" s="18">
         <v>500</v>
@@ -3195,12 +3207,12 @@
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="14"/>
       <c r="G87" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H87" s="18">
         <v>500</v>
@@ -3216,12 +3228,12 @@
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="14"/>
       <c r="G88" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H88" s="18">
         <v>500</v>
@@ -3237,12 +3249,12 @@
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
       <c r="D89" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="14"/>
       <c r="G89" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H89" s="18">
         <v>500</v>
@@ -3258,12 +3270,12 @@
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E90" s="13"/>
       <c r="F90" s="14"/>
       <c r="G90" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H90" s="18">
         <v>500</v>
@@ -3279,14 +3291,14 @@
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="14" t="s">
-        <v>158</v>
+        <v>246</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H91" s="18">
         <v>1500</v>
@@ -3302,12 +3314,12 @@
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
       <c r="D92" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E92" s="13"/>
       <c r="F92" s="14"/>
       <c r="G92" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H92" s="18">
         <v>550</v>
@@ -3323,12 +3335,12 @@
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E93" s="13"/>
       <c r="F93" s="14"/>
       <c r="G93" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H93" s="18">
         <v>550</v>
@@ -3344,12 +3356,12 @@
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
       <c r="D94" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E94" s="13"/>
       <c r="F94" s="14"/>
       <c r="G94" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H94" s="18">
         <v>550</v>
@@ -3365,12 +3377,12 @@
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E95" s="13"/>
       <c r="F95" s="14"/>
       <c r="G95" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H95" s="18">
         <v>550</v>
@@ -3386,14 +3398,14 @@
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E96" s="13"/>
       <c r="F96" s="14" t="s">
-        <v>158</v>
+        <v>247</v>
       </c>
       <c r="G96" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H96" s="18">
         <v>2000</v>
@@ -3409,12 +3421,12 @@
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E97" s="13"/>
       <c r="F97" s="14"/>
       <c r="G97" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H97" s="18">
         <v>600</v>
@@ -3430,12 +3442,12 @@
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
       <c r="D98" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E98" s="13"/>
       <c r="F98" s="14"/>
       <c r="G98" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H98" s="18">
         <v>600</v>
@@ -3451,12 +3463,12 @@
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E99" s="13"/>
       <c r="F99" s="14"/>
       <c r="G99" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H99" s="18">
         <v>600</v>
@@ -3472,12 +3484,12 @@
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E100" s="13"/>
       <c r="F100" s="14"/>
       <c r="G100" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H100" s="18">
         <v>600</v>
@@ -3493,14 +3505,14 @@
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="14" t="s">
-        <v>114</v>
+        <v>244</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H101" s="18">
         <v>2500</v>
@@ -3516,16 +3528,16 @@
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
       <c r="D102" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>114</v>
+        <v>243</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H102" s="18">
         <v>10</v>
@@ -3534,57 +3546,59 @@
         <v>700</v>
       </c>
     </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="H103" s="19">
+        <f>AVERAGE(H2:H102)</f>
+        <v>395.89108910891088</v>
+      </c>
+      <c r="I103" s="19">
+        <f>AVERAGE(I2:I102)</f>
+        <v>100.34653465346534</v>
+      </c>
+    </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F104" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="G104" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H104" s="19">
-        <f>AVERAGE(H2:H102)</f>
-        <v>395.89108910891088</v>
-      </c>
-      <c r="I104" s="19">
-        <f>AVERAGE(I2:I102)</f>
-        <v>100.34653465346534</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to layout plans for the levels
--cores were nerfed to make more playable in the endless modes
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
+++ b/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="283">
   <si>
     <t>LevelName</t>
   </si>
@@ -384,36 +384,21 @@
     <t>5</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
     <t>Slots/Wave</t>
   </si>
   <si>
-    <t>+2 per wave</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -666,18 +651,6 @@
     <t>20,21,22,23,26</t>
   </si>
   <si>
-    <t>15,18,19,20,25</t>
-  </si>
-  <si>
-    <t>7,8,9,10,20</t>
-  </si>
-  <si>
-    <t>10,14,17,19</t>
-  </si>
-  <si>
-    <t>10,15,16,19,24,28</t>
-  </si>
-  <si>
     <t>3,7,9</t>
   </si>
   <si>
@@ -690,15 +663,9 @@
     <t>15,18,20,22</t>
   </si>
   <si>
-    <t>10,11,12,13,14</t>
-  </si>
-  <si>
     <t>18,19,20.21</t>
   </si>
   <si>
-    <t>5,6,14,15,20,21,27,30</t>
-  </si>
-  <si>
     <t>All armored</t>
   </si>
   <si>
@@ -720,9 +687,6 @@
     <t>all shields</t>
   </si>
   <si>
-    <t>18,19,20,23,27</t>
-  </si>
-  <si>
     <t>Mix ultamates/buff</t>
   </si>
   <si>
@@ -744,12 +708,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>treat 1 as 4 waves</t>
-  </si>
-  <si>
-    <t>10,11,15,16,25,26,30</t>
-  </si>
-  <si>
     <t>Ernesto</t>
   </si>
   <si>
@@ -766,6 +724,150 @@
   </si>
   <si>
     <t>Gigantodon</t>
+  </si>
+  <si>
+    <t>15,16,25,26,30</t>
+  </si>
+  <si>
+    <t>16,24,28</t>
+  </si>
+  <si>
+    <t>18,23,27</t>
+  </si>
+  <si>
+    <t>19,20,25</t>
+  </si>
+  <si>
+    <t>7,8,9,20</t>
+  </si>
+  <si>
+    <t>17,19</t>
+  </si>
+  <si>
+    <t>5,14,20,27,30</t>
+  </si>
+  <si>
+    <t>10,12,14</t>
+  </si>
+  <si>
+    <t>18,19,20</t>
+  </si>
+  <si>
+    <t>15,20,25</t>
+  </si>
+  <si>
+    <t>25,30</t>
+  </si>
+  <si>
+    <t>20,22,24,26</t>
+  </si>
+  <si>
+    <t>25,26,27</t>
+  </si>
+  <si>
+    <t>13,16,19</t>
+  </si>
+  <si>
+    <t>15,19,23</t>
+  </si>
+  <si>
+    <t>25,30,31,32</t>
+  </si>
+  <si>
+    <t>13,15,17</t>
+  </si>
+  <si>
+    <t>8,10,20,22</t>
+  </si>
+  <si>
+    <t>8,10,12</t>
+  </si>
+  <si>
+    <t>15,16,20</t>
+  </si>
+  <si>
+    <t>25,26</t>
+  </si>
+  <si>
+    <t>13,16,17,23</t>
+  </si>
+  <si>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>8,15,16,27</t>
+  </si>
+  <si>
+    <t>18,19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>8, 23,28</t>
+  </si>
+  <si>
+    <t>13,15,30,35</t>
+  </si>
+  <si>
+    <t>5,10,35</t>
+  </si>
+  <si>
+    <t>4,6,8,10,18</t>
+  </si>
+  <si>
+    <t>10,20,21,22</t>
+  </si>
+  <si>
+    <t>18,25</t>
+  </si>
+  <si>
+    <t>19,26,27</t>
+  </si>
+  <si>
+    <t>18,21</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>16,17,18,19</t>
+  </si>
+  <si>
+    <t>7,19</t>
+  </si>
+  <si>
+    <t>14,16,23,25,30</t>
+  </si>
+  <si>
+    <t>19,20,21,24</t>
+  </si>
+  <si>
+    <t>30,35</t>
+  </si>
+  <si>
+    <t>18, 22,24</t>
+  </si>
+  <si>
+    <t>18,19,25,26</t>
+  </si>
+  <si>
+    <t>21,25,27</t>
+  </si>
+  <si>
+    <t>27,30</t>
+  </si>
+  <si>
+    <t>30,31</t>
+  </si>
+  <si>
+    <t>24,25,28</t>
+  </si>
+  <si>
+    <t>4,10,16,24,30</t>
+  </si>
+  <si>
+    <t>5,10,15,20,25,30</t>
   </si>
 </sst>
 </file>
@@ -1210,9 +1312,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1245,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>108</v>
@@ -1254,10 +1356,10 @@
         <v>2</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="21"/>
@@ -1274,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="12" t="s">
@@ -1300,7 +1402,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
@@ -1324,11 +1426,11 @@
         <v>116</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H4" s="17">
         <v>100</v>
@@ -1348,11 +1450,11 @@
         <v>116</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H5" s="17">
         <v>100</v>
@@ -1368,17 +1470,17 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H6" s="17">
         <v>110</v>
@@ -1398,11 +1500,11 @@
         <v>118</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H7" s="17">
         <v>110</v>
@@ -1418,17 +1520,17 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>116</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H8" s="17">
         <v>110</v>
@@ -1448,11 +1550,11 @@
         <v>116</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H9" s="17">
         <v>120</v>
@@ -1472,11 +1574,11 @@
         <v>116</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H10" s="17">
         <v>120</v>
@@ -1496,13 +1598,13 @@
         <v>119</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H11" s="17">
         <v>500</v>
@@ -1522,11 +1624,11 @@
         <v>116</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H12" s="17">
         <v>130</v>
@@ -1546,11 +1648,11 @@
         <v>118</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H13" s="17">
         <v>130</v>
@@ -1570,11 +1672,11 @@
         <v>118</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H14" s="17">
         <v>130</v>
@@ -1590,17 +1692,17 @@
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H15" s="17">
         <v>130</v>
@@ -1620,11 +1722,11 @@
         <v>116</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="12" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H16" s="17">
         <v>140</v>
@@ -1644,11 +1746,11 @@
         <v>118</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H17" s="17">
         <v>140</v>
@@ -1668,11 +1770,11 @@
         <v>116</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="12" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H18" s="17">
         <v>140</v>
@@ -1692,11 +1794,11 @@
         <v>117</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H19" s="17">
         <v>140</v>
@@ -1716,11 +1818,11 @@
         <v>119</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H20" s="17">
         <v>140</v>
@@ -1736,19 +1838,19 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>116</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H21" s="17">
         <v>500</v>
@@ -1768,11 +1870,11 @@
         <v>118</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="12" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H22" s="17">
         <v>150</v>
@@ -1792,11 +1894,11 @@
         <v>118</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H23" s="17">
         <v>150</v>
@@ -1816,11 +1918,11 @@
         <v>116</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="12" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H24" s="17">
         <v>150</v>
@@ -1840,11 +1942,11 @@
         <v>119</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H25" s="17">
         <v>150</v>
@@ -1864,13 +1966,13 @@
         <v>120</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H26" s="17">
         <v>700</v>
@@ -1886,17 +1988,17 @@
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>116</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="25" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H27" s="26">
         <v>120</v>
@@ -1916,11 +2018,11 @@
         <v>118</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="25" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="H28" s="26">
         <v>120</v>
@@ -1940,11 +2042,11 @@
         <v>119</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="25" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H29" s="26">
         <v>120</v>
@@ -1964,11 +2066,11 @@
         <v>119</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="25" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="H30" s="26">
         <v>120</v>
@@ -1988,7 +2090,7 @@
         <v>118</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="25"/>
@@ -2006,17 +2108,17 @@
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="23" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>116</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="25" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="H32" s="26">
         <v>120</v>
@@ -2036,7 +2138,7 @@
         <v>116</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="25"/>
@@ -2058,7 +2160,7 @@
         <v>118</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="25"/>
@@ -2076,17 +2178,17 @@
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>116</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="25" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="H35" s="26">
         <v>130</v>
@@ -2103,16 +2205,16 @@
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="H36" s="26">
         <v>500</v>
@@ -2128,17 +2230,17 @@
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>119</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="25" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H37" s="26">
         <v>150</v>
@@ -2158,7 +2260,7 @@
         <v>118</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="25"/>
@@ -2180,7 +2282,7 @@
         <v>119</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="25"/>
@@ -2202,7 +2304,7 @@
         <v>118</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="25"/>
@@ -2224,7 +2326,7 @@
         <v>120</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>111</v>
@@ -2244,17 +2346,17 @@
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="23" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="25" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="H42" s="26">
         <v>160</v>
@@ -2271,10 +2373,10 @@
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="25"/>
@@ -2293,13 +2395,13 @@
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
       <c r="D44" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="G44" s="25"/>
       <c r="H44" s="26">
@@ -2317,10 +2419,10 @@
       <c r="B45" s="23"/>
       <c r="C45" s="23"/>
       <c r="D45" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="25"/>
@@ -2339,10 +2441,10 @@
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>112</v>
@@ -2366,7 +2468,7 @@
         <v>118</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="25"/>
@@ -2388,7 +2490,7 @@
         <v>120</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="25"/>
@@ -2410,7 +2512,7 @@
         <v>119</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="25"/>
@@ -2429,10 +2531,10 @@
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
       <c r="D50" s="23" t="s">
-        <v>241</v>
+        <v>117</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="25"/>
@@ -2451,10 +2553,10 @@
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
       <c r="D51" s="23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>113</v>
@@ -2478,7 +2580,7 @@
         <v>119</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="25"/>
@@ -2497,10 +2599,10 @@
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
       <c r="D53" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="25"/>
@@ -2522,7 +2624,7 @@
         <v>119</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="25"/>
@@ -2544,7 +2646,7 @@
         <v>119</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="25"/>
@@ -2563,13 +2665,13 @@
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
       <c r="D56" s="23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="26">
@@ -2587,9 +2689,11 @@
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E57" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>243</v>
+      </c>
       <c r="F57" s="14"/>
       <c r="G57" s="15"/>
       <c r="H57" s="18">
@@ -2606,9 +2710,11 @@
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E58" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>244</v>
+      </c>
       <c r="F58" s="14"/>
       <c r="G58" s="15"/>
       <c r="H58" s="18">
@@ -2625,9 +2731,11 @@
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E59" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>245</v>
+      </c>
       <c r="F59" s="14"/>
       <c r="G59" s="15"/>
       <c r="H59" s="18">
@@ -2646,7 +2754,9 @@
       <c r="D60" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="13"/>
+      <c r="E60" s="13" t="s">
+        <v>246</v>
+      </c>
       <c r="F60" s="14"/>
       <c r="G60" s="15"/>
       <c r="H60" s="18">
@@ -2663,9 +2773,11 @@
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>247</v>
+      </c>
       <c r="F61" s="14"/>
       <c r="G61" s="15"/>
       <c r="H61" s="18">
@@ -2682,9 +2794,11 @@
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
       <c r="D62" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E62" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F62" s="14"/>
       <c r="G62" s="15"/>
       <c r="H62" s="18">
@@ -2701,9 +2815,11 @@
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
       <c r="D63" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E63" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>248</v>
+      </c>
       <c r="F63" s="14"/>
       <c r="G63" s="15"/>
       <c r="H63" s="18">
@@ -2720,9 +2836,11 @@
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E64" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>200</v>
+      </c>
       <c r="F64" s="14"/>
       <c r="G64" s="15"/>
       <c r="H64" s="18">
@@ -2739,9 +2857,11 @@
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E65" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>249</v>
+      </c>
       <c r="F65" s="14"/>
       <c r="G65" s="15"/>
       <c r="H65" s="18">
@@ -2758,11 +2878,13 @@
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E66" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>250</v>
+      </c>
       <c r="F66" s="14" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="18">
@@ -2779,9 +2901,11 @@
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>251</v>
+      </c>
       <c r="F67" s="14"/>
       <c r="G67" s="15"/>
       <c r="H67" s="18">
@@ -2798,9 +2922,11 @@
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>252</v>
+      </c>
       <c r="F68" s="14"/>
       <c r="G68" s="15"/>
       <c r="H68" s="18">
@@ -2815,15 +2941,17 @@
         <v>74</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="F69" s="14"/>
       <c r="G69" s="15" t="s">
         <v>7</v>
@@ -2840,15 +2968,17 @@
         <v>75</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D70" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E70" s="13"/>
+      <c r="E70" s="13" t="s">
+        <v>253</v>
+      </c>
       <c r="F70" s="14"/>
       <c r="G70" s="15"/>
       <c r="H70" s="18">
@@ -2867,12 +2997,14 @@
       <c r="D71" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E71" s="13"/>
+      <c r="E71" s="13" t="s">
+        <v>262</v>
+      </c>
       <c r="F71" s="14" t="s">
         <v>114</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H71" s="18">
         <v>1000</v>
@@ -2888,12 +3020,14 @@
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E72" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>245</v>
+      </c>
       <c r="F72" s="14"/>
       <c r="G72" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H72" s="18">
         <v>450</v>
@@ -2909,12 +3043,14 @@
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E73" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="F73" s="14"/>
       <c r="G73" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H73" s="18">
         <v>450</v>
@@ -2930,12 +3066,14 @@
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E74" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>255</v>
+      </c>
       <c r="F74" s="14"/>
       <c r="G74" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H74" s="18">
         <v>450</v>
@@ -2953,10 +3091,12 @@
       <c r="D75" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="13"/>
+      <c r="E75" s="13" t="s">
+        <v>256</v>
+      </c>
       <c r="F75" s="14"/>
       <c r="G75" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H75" s="18">
         <v>450</v>
@@ -2974,12 +3114,14 @@
       <c r="D76" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E76" s="13"/>
+      <c r="E76" s="13" t="s">
+        <v>261</v>
+      </c>
       <c r="F76" s="14" t="s">
         <v>115</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H76" s="18">
         <v>1300</v>
@@ -2995,12 +3137,14 @@
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E77" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>257</v>
+      </c>
       <c r="F77" s="14"/>
       <c r="G77" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H77" s="18">
         <v>450</v>
@@ -3016,12 +3160,14 @@
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
       <c r="D78" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E78" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>258</v>
+      </c>
       <c r="F78" s="14"/>
       <c r="G78" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H78" s="18">
         <v>450</v>
@@ -3037,12 +3183,14 @@
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E79" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>259</v>
+      </c>
       <c r="F79" s="14"/>
       <c r="G79" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H79" s="18">
         <v>450</v>
@@ -3058,12 +3206,14 @@
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
       <c r="D80" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E80" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>260</v>
+      </c>
       <c r="F80" s="14"/>
       <c r="G80" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H80" s="18">
         <v>450</v>
@@ -3079,14 +3229,16 @@
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
       <c r="D81" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E81" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>263</v>
+      </c>
       <c r="F81" s="14" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H81" s="18">
         <v>1800</v>
@@ -3102,12 +3254,14 @@
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E82" s="13"/>
+        <v>120</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>264</v>
+      </c>
       <c r="F82" s="14"/>
       <c r="G82" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H82" s="18">
         <v>500</v>
@@ -3125,10 +3279,12 @@
       <c r="D83" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E83" s="13"/>
+      <c r="E83" s="13" t="s">
+        <v>265</v>
+      </c>
       <c r="F83" s="14"/>
       <c r="G83" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H83" s="18">
         <v>500</v>
@@ -3144,12 +3300,14 @@
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
       <c r="D84" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E84" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="F84" s="14"/>
       <c r="G84" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H84" s="18">
         <v>500</v>
@@ -3165,12 +3323,14 @@
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E85" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>267</v>
+      </c>
       <c r="F85" s="14"/>
       <c r="G85" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H85" s="18">
         <v>500</v>
@@ -3186,12 +3346,14 @@
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E86" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>268</v>
+      </c>
       <c r="F86" s="14"/>
       <c r="G86" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H86" s="18">
         <v>500</v>
@@ -3207,12 +3369,14 @@
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E87" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>245</v>
+      </c>
       <c r="F87" s="14"/>
       <c r="G87" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H87" s="18">
         <v>500</v>
@@ -3228,12 +3392,14 @@
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E88" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>269</v>
+      </c>
       <c r="F88" s="14"/>
       <c r="G88" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H88" s="18">
         <v>500</v>
@@ -3249,12 +3415,14 @@
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
       <c r="D89" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E89" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>270</v>
+      </c>
       <c r="F89" s="14"/>
       <c r="G89" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H89" s="18">
         <v>500</v>
@@ -3270,12 +3438,14 @@
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E90" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="F90" s="14"/>
       <c r="G90" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H90" s="18">
         <v>500</v>
@@ -3291,14 +3461,16 @@
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E91" s="13"/>
+        <v>120</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="F91" s="14" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H91" s="18">
         <v>1500</v>
@@ -3316,10 +3488,12 @@
       <c r="D92" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E92" s="13"/>
+      <c r="E92" s="13" t="s">
+        <v>273</v>
+      </c>
       <c r="F92" s="14"/>
       <c r="G92" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H92" s="18">
         <v>550</v>
@@ -3337,10 +3511,12 @@
       <c r="D93" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E93" s="13"/>
+      <c r="E93" s="13" t="s">
+        <v>274</v>
+      </c>
       <c r="F93" s="14"/>
       <c r="G93" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H93" s="18">
         <v>550</v>
@@ -3358,10 +3534,12 @@
       <c r="D94" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E94" s="13"/>
+      <c r="E94" s="13" t="s">
+        <v>275</v>
+      </c>
       <c r="F94" s="14"/>
       <c r="G94" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H94" s="18">
         <v>550</v>
@@ -3377,12 +3555,14 @@
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E95" s="13"/>
+        <v>119</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>276</v>
+      </c>
       <c r="F95" s="14"/>
       <c r="G95" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H95" s="18">
         <v>550</v>
@@ -3398,14 +3578,16 @@
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E96" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>277</v>
+      </c>
       <c r="F96" s="14" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G96" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H96" s="18">
         <v>2000</v>
@@ -3421,12 +3603,14 @@
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E97" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>278</v>
+      </c>
       <c r="F97" s="14"/>
       <c r="G97" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H97" s="18">
         <v>600</v>
@@ -3442,12 +3626,14 @@
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
       <c r="D98" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E98" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>202</v>
+      </c>
       <c r="F98" s="14"/>
       <c r="G98" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H98" s="18">
         <v>600</v>
@@ -3463,12 +3649,14 @@
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E99" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="F99" s="14"/>
       <c r="G99" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H99" s="18">
         <v>600</v>
@@ -3484,12 +3672,14 @@
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E100" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>280</v>
+      </c>
       <c r="F100" s="14"/>
       <c r="G100" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H100" s="18">
         <v>600</v>
@@ -3505,14 +3695,16 @@
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E101" s="13"/>
+        <v>120</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>281</v>
+      </c>
       <c r="F101" s="14" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H101" s="18">
         <v>2500</v>
@@ -3528,16 +3720,16 @@
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
       <c r="D102" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H102" s="18">
         <v>10</v>
@@ -3558,47 +3750,47 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
world 2 level enemies list set
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
+++ b/BombShootDown/Assets/Templates/Levels/LevelDesign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="339">
   <si>
     <t>LevelName</t>
   </si>
@@ -690,9 +690,6 @@
     <t>all buffers, ultimates, megas</t>
   </si>
   <si>
-    <t>ultimates, gigas, zippers</t>
-  </si>
-  <si>
     <t>all basic, armored, shileded; vessel, meso vessel</t>
   </si>
   <si>
@@ -918,9 +915,6 @@
     <t>Maintainers, Protectors, base/meso/macro tickers, Gigas &amp; Ultimates</t>
   </si>
   <si>
-    <t>Havocs, Zippers, Shifters, up to Kilos</t>
-  </si>
-  <si>
     <t>base/meso engima &amp; reflector &amp; Outlier, All Sheilds/Armored</t>
   </si>
   <si>
@@ -945,24 +939,15 @@
     <t>Macro &amp; Hyper tickers, Macro &amp; Hyper Outliers,  base/meso/macro shifters</t>
   </si>
   <si>
-    <t>Shifters</t>
-  </si>
-  <si>
     <t>HyperHavocs &amp; ticker</t>
   </si>
   <si>
-    <t>carriers</t>
-  </si>
-  <si>
     <t>All basic available, mesocarriers</t>
   </si>
   <si>
     <t>All basic available, mesocores</t>
   </si>
   <si>
-    <t xml:space="preserve">cores, </t>
-  </si>
-  <si>
     <t>All basic available 2 mesocores  &amp; 2 mesocarriers at once.</t>
   </si>
   <si>
@@ -970,6 +955,87 @@
   </si>
   <si>
     <t>Ultimates, HyperTicker/Teleporters</t>
+  </si>
+  <si>
+    <t>MacroVessel, MacroTeleporter</t>
+  </si>
+  <si>
+    <t>all shifters</t>
+  </si>
+  <si>
+    <t>reflectors up to macro, gigas</t>
+  </si>
+  <si>
+    <t>maintainer, protector, shields</t>
+  </si>
+  <si>
+    <t>cores, armory, armored</t>
+  </si>
+  <si>
+    <t>carriers, outliers up to macro, zippers up to macro</t>
+  </si>
+  <si>
+    <t>macro tickers, engimas up to macro, booster</t>
+  </si>
+  <si>
+    <t>jammer, vessel up to macro, basic types</t>
+  </si>
+  <si>
+    <t>all basics</t>
+  </si>
+  <si>
+    <t>enigma up to macro, zipper up to macro, only base type</t>
+  </si>
+  <si>
+    <t>disruptor, zippers, shifter (to macro)</t>
+  </si>
+  <si>
+    <t>All basic available, hyp havoc</t>
+  </si>
+  <si>
+    <t>All basic available, hyp protector</t>
+  </si>
+  <si>
+    <t>All basic available, hyp booster</t>
+  </si>
+  <si>
+    <t>All basic available. Hyp maintainer</t>
+  </si>
+  <si>
+    <t>All basic available, hyp armory</t>
+  </si>
+  <si>
+    <t>All basic available, hyp jammer</t>
+  </si>
+  <si>
+    <t>All basic available, hyp disruptor</t>
+  </si>
+  <si>
+    <t>All basic available, hyp disruptor &amp; jammer</t>
+  </si>
+  <si>
+    <t>carrier, core, basic types up to kilo</t>
+  </si>
+  <si>
+    <t>All basic available, all buff/debuff</t>
+  </si>
+  <si>
+    <t>All basic available, hyp protector, armory, maintainer, disruptor</t>
+  </si>
+  <si>
+    <t>All basic available, hyp havoc, booster, jammer</t>
+  </si>
+  <si>
+    <t>All basic available, all the non hyper buffers/debuffer</t>
+  </si>
+  <si>
+    <t>tickers, enigmas</t>
+  </si>
+  <si>
+    <t>ultimates, gigas, base/meso zipper</t>
+  </si>
+  <si>
+    <t>Havocs, Zippers, Shifters - up to macros</t>
   </si>
 </sst>
 </file>
@@ -1414,9 +1480,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2196,7 +2262,7 @@
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H31" s="26">
         <v>120</v>
@@ -2222,7 +2288,7 @@
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H32" s="26">
         <v>120</v>
@@ -2246,7 +2312,7 @@
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H33" s="26">
         <v>130</v>
@@ -2270,7 +2336,7 @@
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H34" s="26">
         <v>130</v>
@@ -2316,7 +2382,7 @@
         <v>118</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>221</v>
@@ -2348,7 +2414,7 @@
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="25" t="s">
-        <v>223</v>
+        <v>337</v>
       </c>
       <c r="H37" s="26">
         <v>150</v>
@@ -2364,7 +2430,7 @@
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>118</v>
@@ -2374,7 +2440,7 @@
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H38" s="26">
         <v>150</v>
@@ -2398,7 +2464,7 @@
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H39" s="26">
         <v>150</v>
@@ -2422,7 +2488,7 @@
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H40" s="26">
         <v>160</v>
@@ -2448,7 +2514,7 @@
         <v>111</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H41" s="26">
         <v>600</v>
@@ -2474,7 +2540,7 @@
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H42" s="26">
         <v>160</v>
@@ -2494,11 +2560,11 @@
         <v>118</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H43" s="26">
         <v>170</v>
@@ -2518,13 +2584,13 @@
         <v>119</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H44" s="26">
         <v>170</v>
@@ -2544,11 +2610,11 @@
         <v>116</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H45" s="26">
         <v>170</v>
@@ -2568,13 +2634,13 @@
         <v>118</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>112</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H46" s="26">
         <v>700</v>
@@ -2598,7 +2664,7 @@
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H47" s="26">
         <v>180</v>
@@ -2622,7 +2688,7 @@
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H48" s="26">
         <v>180</v>
@@ -2646,7 +2712,7 @@
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H49" s="26">
         <v>180</v>
@@ -2666,11 +2732,11 @@
         <v>117</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H50" s="26">
         <v>180</v>
@@ -2690,13 +2756,13 @@
         <v>120</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>113</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H51" s="26">
         <v>800</v>
@@ -2720,7 +2786,7 @@
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H52" s="26">
         <v>200</v>
@@ -2740,11 +2806,11 @@
         <v>118</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H53" s="26">
         <v>200</v>
@@ -2768,7 +2834,7 @@
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H54" s="26">
         <v>225</v>
@@ -2792,7 +2858,7 @@
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="25" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="H55" s="26">
         <v>225</v>
@@ -2812,13 +2878,13 @@
         <v>120</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H56" s="26">
         <v>1000</v>
@@ -2838,10 +2904,12 @@
         <v>118</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F57" s="14"/>
-      <c r="G57" s="15"/>
+      <c r="G57" s="15" t="s">
+        <v>320</v>
+      </c>
       <c r="H57" s="18">
         <v>250</v>
       </c>
@@ -2859,10 +2927,12 @@
         <v>118</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F58" s="14"/>
-      <c r="G58" s="15"/>
+      <c r="G58" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="H58" s="18">
         <v>250</v>
       </c>
@@ -2880,10 +2950,12 @@
         <v>116</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F59" s="14"/>
-      <c r="G59" s="15"/>
+      <c r="G59" s="15" t="s">
+        <v>318</v>
+      </c>
       <c r="H59" s="18">
         <v>275</v>
       </c>
@@ -2901,11 +2973,11 @@
         <v>119</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F60" s="14"/>
       <c r="G60" s="15" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="H60" s="18">
         <v>275</v>
@@ -2924,10 +2996,12 @@
         <v>118</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F61" s="14"/>
-      <c r="G61" s="15"/>
+      <c r="G61" s="15" t="s">
+        <v>321</v>
+      </c>
       <c r="H61" s="18">
         <v>275</v>
       </c>
@@ -2949,7 +3023,7 @@
       </c>
       <c r="F62" s="14"/>
       <c r="G62" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H62" s="18">
         <v>300</v>
@@ -2968,10 +3042,12 @@
         <v>118</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F63" s="14"/>
-      <c r="G63" s="15"/>
+      <c r="G63" s="15" t="s">
+        <v>322</v>
+      </c>
       <c r="H63" s="18">
         <v>300</v>
       </c>
@@ -2992,7 +3068,9 @@
         <v>200</v>
       </c>
       <c r="F64" s="14"/>
-      <c r="G64" s="15"/>
+      <c r="G64" s="15" t="s">
+        <v>314</v>
+      </c>
       <c r="H64" s="18">
         <v>325</v>
       </c>
@@ -3010,11 +3088,11 @@
         <v>118</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="15" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H65" s="18">
         <v>325</v>
@@ -3033,13 +3111,13 @@
         <v>119</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H66" s="18">
         <v>1200</v>
@@ -3058,10 +3136,12 @@
         <v>118</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F67" s="14"/>
-      <c r="G67" s="15"/>
+      <c r="G67" s="15" t="s">
+        <v>315</v>
+      </c>
       <c r="H67" s="18">
         <v>325</v>
       </c>
@@ -3079,10 +3159,12 @@
         <v>119</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F68" s="14"/>
-      <c r="G68" s="15"/>
+      <c r="G68" s="15" t="s">
+        <v>312</v>
+      </c>
       <c r="H68" s="18">
         <v>325</v>
       </c>
@@ -3131,11 +3213,11 @@
         <v>118</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="15" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H70" s="18">
         <v>350</v>
@@ -3154,7 +3236,7 @@
         <v>119</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>114</v>
@@ -3179,11 +3261,11 @@
         <v>116</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F72" s="14"/>
       <c r="G72" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H72" s="18">
         <v>450</v>
@@ -3202,7 +3284,7 @@
         <v>118</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F73" s="14"/>
       <c r="G73" s="15" t="s">
@@ -3225,7 +3307,7 @@
         <v>116</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F74" s="14"/>
       <c r="G74" s="15" t="s">
@@ -3248,11 +3330,11 @@
         <v>119</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F75" s="14"/>
       <c r="G75" s="15" t="s">
-        <v>151</v>
+        <v>323</v>
       </c>
       <c r="H75" s="18">
         <v>450</v>
@@ -3271,7 +3353,7 @@
         <v>118</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>115</v>
@@ -3296,11 +3378,11 @@
         <v>116</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F77" s="14"/>
       <c r="G77" s="15" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="H77" s="18">
         <v>450</v>
@@ -3319,11 +3401,11 @@
         <v>119</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="15" t="s">
-        <v>151</v>
+        <v>324</v>
       </c>
       <c r="H78" s="18">
         <v>450</v>
@@ -3342,11 +3424,11 @@
         <v>116</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F79" s="14"/>
       <c r="G79" s="15" t="s">
-        <v>151</v>
+        <v>325</v>
       </c>
       <c r="H79" s="18">
         <v>450</v>
@@ -3365,7 +3447,7 @@
         <v>117</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F80" s="14"/>
       <c r="G80" s="15" t="s">
@@ -3388,10 +3470,10 @@
         <v>118</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>151</v>
@@ -3413,11 +3495,11 @@
         <v>120</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F82" s="14"/>
       <c r="G82" s="15" t="s">
-        <v>151</v>
+        <v>326</v>
       </c>
       <c r="H82" s="18">
         <v>500</v>
@@ -3436,11 +3518,11 @@
         <v>119</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F83" s="14"/>
       <c r="G83" s="15" t="s">
-        <v>151</v>
+        <v>327</v>
       </c>
       <c r="H83" s="18">
         <v>500</v>
@@ -3459,11 +3541,11 @@
         <v>116</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F84" s="14"/>
       <c r="G84" s="15" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H84" s="18">
         <v>500</v>
@@ -3482,11 +3564,11 @@
         <v>118</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F85" s="14"/>
       <c r="G85" s="15" t="s">
-        <v>151</v>
+        <v>328</v>
       </c>
       <c r="H85" s="18">
         <v>500</v>
@@ -3505,11 +3587,11 @@
         <v>116</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F86" s="14"/>
       <c r="G86" s="15" t="s">
-        <v>151</v>
+        <v>329</v>
       </c>
       <c r="H86" s="18">
         <v>500</v>
@@ -3528,11 +3610,11 @@
         <v>116</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F87" s="14"/>
       <c r="G87" s="15" t="s">
-        <v>151</v>
+        <v>330</v>
       </c>
       <c r="H87" s="18">
         <v>500</v>
@@ -3551,10 +3633,12 @@
         <v>116</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F88" s="14"/>
-      <c r="G88" s="15"/>
+      <c r="G88" s="15" t="s">
+        <v>331</v>
+      </c>
       <c r="H88" s="18">
         <v>500</v>
       </c>
@@ -3572,7 +3656,7 @@
         <v>119</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F89" s="14"/>
       <c r="G89" s="15" t="s">
@@ -3595,10 +3679,12 @@
         <v>116</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F90" s="14"/>
-      <c r="G90" s="15"/>
+      <c r="G90" s="15" t="s">
+        <v>336</v>
+      </c>
       <c r="H90" s="18">
         <v>500</v>
       </c>
@@ -3616,10 +3702,10 @@
         <v>120</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G91" s="15" t="s">
         <v>151</v>
@@ -3641,7 +3727,7 @@
         <v>119</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F92" s="14"/>
       <c r="G92" s="15" t="s">
@@ -3664,11 +3750,11 @@
         <v>116</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F93" s="14"/>
       <c r="G93" s="15" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
       <c r="H93" s="18">
         <v>550</v>
@@ -3687,7 +3773,7 @@
         <v>118</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F94" s="14"/>
       <c r="G94" s="15" t="s">
@@ -3710,11 +3796,11 @@
         <v>119</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F95" s="14"/>
       <c r="G95" s="15" t="s">
-        <v>151</v>
+        <v>334</v>
       </c>
       <c r="H95" s="18">
         <v>550</v>
@@ -3733,13 +3819,13 @@
         <v>118</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F96" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="G96" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="G96" s="15" t="s">
-        <v>306</v>
       </c>
       <c r="H96" s="18">
         <v>2000</v>
@@ -3758,11 +3844,11 @@
         <v>116</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F97" s="14"/>
       <c r="G97" s="15" t="s">
-        <v>151</v>
+        <v>332</v>
       </c>
       <c r="H97" s="18">
         <v>600</v>
@@ -3785,7 +3871,7 @@
       </c>
       <c r="F98" s="14"/>
       <c r="G98" s="15" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="H98" s="18">
         <v>600</v>
@@ -3804,11 +3890,11 @@
         <v>116</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F99" s="14"/>
       <c r="G99" s="15" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H99" s="18">
         <v>600</v>
@@ -3827,11 +3913,11 @@
         <v>118</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F100" s="14"/>
       <c r="G100" s="15" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H100" s="18">
         <v>600</v>
@@ -3850,13 +3936,13 @@
         <v>120</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H101" s="18">
         <v>2500</v>
@@ -3875,13 +3961,13 @@
         <v>121</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H102" s="18">
         <v>10</v>
@@ -3914,7 +4000,7 @@
         <v>128</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.5">
@@ -3931,7 +4017,7 @@
         <v>133</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.5">
@@ -3948,7 +4034,7 @@
         <v>134</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>